<commit_message>
USB Hub Switch Updates
</commit_message>
<xml_diff>
--- a/Switches/USB Hub Switch/Electronics/BOM_USBHubSmartSwitchV300.xlsx
+++ b/Switches/USB Hub Switch/Electronics/BOM_USBHubSmartSwitchV300.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
   <si>
     <t>No.</t>
   </si>
@@ -217,7 +217,7 @@
     <t>10kΩ</t>
   </si>
   <si>
-    <t>R1,R3,R4,R5,R6,R18,R19,R20,R21,R22,R23,R24,R25,R33,R34,R35,R36,R37</t>
+    <t>R1,R3,R4,R5,R6,R18,R19,R20,R21,R22,R23,R24,R25,R33,R34,R35,R36</t>
   </si>
   <si>
     <t>R0603</t>
@@ -283,19 +283,16 @@
     <t>14</t>
   </si>
   <si>
-    <t>SS12D07VG4</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>SW-TH_SS12D07VG4</t>
-  </si>
-  <si>
-    <t>HanElectricity(瀚源)</t>
-  </si>
-  <si>
-    <t>C22435633</t>
+    <t>0Ω</t>
+  </si>
+  <si>
+    <t>R37,R38,R39</t>
+  </si>
+  <si>
+    <t>0805W8F0000T5E</t>
+  </si>
+  <si>
+    <t>C17477</t>
   </si>
   <si>
     <t>15</t>
@@ -1150,7 +1147,7 @@
         <v>66</v>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>67</v>
@@ -1278,7 +1275,7 @@
         <v>89</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>90</v>
@@ -1287,19 +1284,19 @@
         <v>91</v>
       </c>
       <c r="E15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" t="s">
         <v>92</v>
       </c>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" t="s">
-        <v>90</v>
-      </c>
       <c r="H15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" t="s">
         <v>93</v>
-      </c>
-      <c r="I15" t="s">
-        <v>94</v>
       </c>
       <c r="J15" t="s">
         <v>17</v>
@@ -1307,31 +1304,31 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" t="s">
         <v>96</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>97</v>
-      </c>
-      <c r="E16" t="s">
-        <v>98</v>
       </c>
       <c r="F16" t="s">
         <v>39</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" t="s">
         <v>99</v>
-      </c>
-      <c r="I16" t="s">
-        <v>100</v>
       </c>
       <c r="J16" t="s">
         <v>17</v>
@@ -1339,31 +1336,31 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" t="s">
         <v>102</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>103</v>
-      </c>
-      <c r="E17" t="s">
-        <v>104</v>
       </c>
       <c r="F17" t="s">
         <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H17" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" t="s">
         <v>105</v>
-      </c>
-      <c r="I17" t="s">
-        <v>106</v>
       </c>
       <c r="J17" t="s">
         <v>17</v>
@@ -1371,31 +1368,31 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
         <v>108</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>109</v>
-      </c>
-      <c r="E18" t="s">
-        <v>110</v>
       </c>
       <c r="F18" t="s">
         <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H18" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" t="s">
         <v>111</v>
-      </c>
-      <c r="I18" t="s">
-        <v>112</v>
       </c>
       <c r="J18" t="s">
         <v>17</v>
@@ -1403,16 +1400,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" t="s">
         <v>114</v>
-      </c>
-      <c r="D19" t="s">
-        <v>115</v>
       </c>
       <c r="E19" t="s">
         <v>57</v>
@@ -1421,13 +1418,13 @@
         <v>39</v>
       </c>
       <c r="G19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H19" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" t="s">
         <v>116</v>
-      </c>
-      <c r="I19" t="s">
-        <v>117</v>
       </c>
       <c r="J19" t="s">
         <v>17</v>
@@ -1435,31 +1432,31 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
       <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
         <v>119</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>120</v>
-      </c>
-      <c r="E20" t="s">
-        <v>121</v>
       </c>
       <c r="F20" t="s">
         <v>39</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H20" t="s">
+        <v>121</v>
+      </c>
+      <c r="I20" t="s">
         <v>122</v>
-      </c>
-      <c r="I20" t="s">
-        <v>123</v>
       </c>
       <c r="J20" t="s">
         <v>17</v>
@@ -1467,31 +1464,31 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" t="s">
         <v>125</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>126</v>
-      </c>
-      <c r="E21" t="s">
-        <v>127</v>
       </c>
       <c r="F21" t="s">
         <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" t="s">
         <v>128</v>
-      </c>
-      <c r="I21" t="s">
-        <v>129</v>
       </c>
       <c r="J21" t="s">
         <v>17</v>
@@ -1499,31 +1496,31 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" t="s">
         <v>131</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>132</v>
-      </c>
-      <c r="E22" t="s">
-        <v>133</v>
       </c>
       <c r="F22" t="s">
         <v>39</v>
       </c>
       <c r="G22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H22" t="s">
+        <v>133</v>
+      </c>
+      <c r="I22" t="s">
         <v>134</v>
-      </c>
-      <c r="I22" t="s">
-        <v>135</v>
       </c>
       <c r="J22" t="s">
         <v>17</v>
@@ -1531,31 +1528,31 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" t="s">
         <v>137</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>138</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" t="s">
         <v>139</v>
       </c>
-      <c r="F23" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>140</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>141</v>
-      </c>
-      <c r="I23" t="s">
-        <v>142</v>
       </c>
       <c r="J23" t="s">
         <v>17</v>

</xml_diff>